<commit_message>
Agregamos al angular los componentes y el servicio
</commit_message>
<xml_diff>
--- a/Documentación/Pruebas.xlsx
+++ b/Documentación/Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\2019\Ingeneria de software\Yaf_inmobiliaria\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE388700-061C-4612-8543-063CF9E96FB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005883E7-D7E0-4AB8-B857-C95A9AD2FFB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3B55A8-782A-4C61-B1F1-439549D0209F}"/>
   </bookViews>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,95 +250,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -363,77 +281,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -749,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9133F45E-A7A0-4C24-A453-28B2794EAF73}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +657,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>28</v>
@@ -892,7 +740,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>30</v>
@@ -912,7 +760,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>30</v>
@@ -932,10 +780,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -952,10 +800,10 @@
         <v>27</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,7 +840,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>30</v>
@@ -1012,7 +860,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>30</v>
@@ -1032,7 +880,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>30</v>
@@ -1059,7 +907,7 @@
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1072,14 +920,14 @@
       <c r="D17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
+      <c r="E17" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1093,14 +941,15 @@
         <v>27</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1114,13 +963,13 @@
         <v>27</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1140,7 +989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1154,13 +1003,13 @@
         <v>27</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1177,23 +1026,23 @@
         <v>28</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$E$4="Aprobado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$E$4="Reprobado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:F22">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$E5="Aprobado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E5="Reprobado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
modificando la parte del excel
</commit_message>
<xml_diff>
--- a/Documentación/Pruebas.xlsx
+++ b/Documentación/Pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\2019\Ingeneria de software\Yaf_inmobiliaria\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Yaf Inmobiliaria\Yaf_inmobiliaria\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005883E7-D7E0-4AB8-B857-C95A9AD2FFB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AA3BC7-B082-4DDC-A208-14FCF7FDE937}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3B55A8-782A-4C61-B1F1-439549D0209F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0B3B55A8-782A-4C61-B1F1-439549D0209F}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas Back-end" sheetId="1" r:id="rId1"/>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9133F45E-A7A0-4C24-A453-28B2794EAF73}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
         <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>